<commit_message>
Update cau_hoi_tra_loi.xlsx with new data
</commit_message>
<xml_diff>
--- a/cau_hoi_tra_loi.xlsx
+++ b/cau_hoi_tra_loi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\ccvc_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B143B0-4FCC-4ADC-BE2A-0395FE87BC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684C54C5-D9C5-45F5-A315-410FD413EE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Câu hỏi mẫu</t>
   </si>
@@ -161,6 +161,33 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1SmFtEEqi8ornKmLl4mZsElW49p4zZkxH/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Lỗi đồng bộ: Đào tạo bôi dưỡng</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1N2fq9B4tWexeeg_0k4n7SO2sqLLlBngS/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Cảnh báo luân chuyển điều động</t>
+  </si>
+  <si>
+    <t>Lỗi không đủ điều kiện đồng bộ: Thông tin gia đình</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1RZIokbEHkGu20Va_Y2A_V-Oh_Y9o1f5r/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Lỗi đồng bộ: Khen thưởng kỷ luật</t>
+  </si>
+  <si>
+    <t>Lỗi đồng bộ: Quan hệ gia đình bản thân không được để trống</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1rBs1Cht1bhUr6Dsue52uU6N3dL5bqM7u/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Cảnh báo không đủ điều kiện đồng bộ: Quốc phòng an ninh, lý luận chính trị, Chuyên môn, quản lý nhà nước</t>
   </si>
 </sst>
 </file>
@@ -535,7 +562,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection sqref="A1:Z1000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1218,8 +1245,12 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1246,8 +1277,12 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1274,8 +1309,12 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1302,8 +1341,12 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
+      <c r="A25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1330,8 +1373,12 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
+      <c r="A26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1357,9 +1404,13 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
+    <row r="27" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -28631,12 +28682,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{86A0769D-ACD6-46EC-98D9-410D998E6598}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{E5A49903-AD2F-4389-B4D8-1CAA191AE40D}"/>
-    <hyperlink ref="B19" r:id="rId3" xr:uid="{E1B1BB9A-A68E-4E19-8E96-9094521AA986}"/>
-    <hyperlink ref="B21" r:id="rId4" xr:uid="{32D66E83-17D1-46CA-ACBA-1B986C06B612}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3B5B2C61-6CC8-4C97-B63C-63FA67188ACC}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{047487BD-8BD8-4937-BD37-1C2A9B26D864}"/>
+    <hyperlink ref="B19" r:id="rId3" xr:uid="{8F98BBBD-DEA4-48A6-862B-0FF172EE628D}"/>
+    <hyperlink ref="B21" r:id="rId4" xr:uid="{98597D4E-5A73-410E-B578-466FF6F6AA39}"/>
+    <hyperlink ref="B22" r:id="rId5" xr:uid="{A91B1F14-9243-48DC-B481-39131DF2378D}"/>
+    <hyperlink ref="B23" r:id="rId6" xr:uid="{D47BC5D5-E367-4445-97E7-98AB86E6FAC4}"/>
+    <hyperlink ref="B24" r:id="rId7" xr:uid="{08AB0D75-D5FD-4C7C-A3E6-4672A7438201}"/>
+    <hyperlink ref="B25" r:id="rId8" xr:uid="{EEE00F80-6E99-4C89-8FD3-056789F10C9F}"/>
+    <hyperlink ref="B26" r:id="rId9" xr:uid="{9F4A5893-E5F9-4C30-8C9C-44C2E74963A2}"/>
+    <hyperlink ref="B27" r:id="rId10" xr:uid="{E4AFC0F1-A2B8-40F3-9A51-98987A653872}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>